<commit_message>
Fixing sorting in part 2 graphs
</commit_message>
<xml_diff>
--- a/part2/part2_answers.xlsx
+++ b/part2/part2_answers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5600" yWindow="0" windowWidth="25360" windowHeight="16180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,8 +221,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,7 +298,7 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
@@ -431,11 +432,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2147177272"/>
-        <c:axId val="-2147422760"/>
+        <c:axId val="-2137851240"/>
+        <c:axId val="-2142288440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2147177272"/>
+        <c:axId val="-2137851240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -465,11 +466,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147422760"/>
+        <c:crossAx val="-2142288440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -477,7 +478,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2147422760"/>
+        <c:axId val="-2142288440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -512,7 +513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147177272"/>
+        <c:crossAx val="-2137851240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -894,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1047,7 +1048,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>4</v>
       </c>
       <c r="D2">
@@ -1151,7 +1152,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>8</v>
       </c>
       <c r="D3">
@@ -1255,7 +1256,7 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>16</v>
       </c>
       <c r="D4">
@@ -1359,7 +1360,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>32</v>
       </c>
       <c r="D5">
@@ -1463,7 +1464,7 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>64</v>
       </c>
       <c r="D6">
@@ -1567,7 +1568,7 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>128</v>
       </c>
       <c r="D7">
@@ -1671,7 +1672,7 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>256</v>
       </c>
       <c r="D8">
@@ -1775,7 +1776,7 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>512</v>
       </c>
       <c r="D9">
@@ -1879,7 +1880,7 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>1024</v>
       </c>
       <c r="D10">
@@ -1983,7 +1984,7 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>2048</v>
       </c>
       <c r="D11">
@@ -2087,7 +2088,7 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>4096</v>
       </c>
       <c r="D12">
@@ -2191,7 +2192,7 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>8192</v>
       </c>
       <c r="D13">
@@ -2295,7 +2296,7 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>16384</v>
       </c>
       <c r="D14">
@@ -2399,7 +2400,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>32768</v>
       </c>
       <c r="D15">
@@ -2503,7 +2504,7 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>65536</v>
       </c>
       <c r="D16">
@@ -2607,7 +2608,7 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="1">
         <v>131072</v>
       </c>
       <c r="D17">
@@ -2711,7 +2712,7 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>262144</v>
       </c>
       <c r="D18">
@@ -2815,7 +2816,7 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>524288</v>
       </c>
       <c r="D19">

</xml_diff>

<commit_message>
Fix adding wrong version of part2_answers.xlsx
</commit_message>
<xml_diff>
--- a/part2/part2_answers.xlsx
+++ b/part2/part2_answers.xlsx
@@ -4,13 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1a" sheetId="1" r:id="rId1"/>
+    <sheet name="2a chunk64" sheetId="2" r:id="rId2"/>
+    <sheet name="2a chunk32" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="merged_part2q1_out" localSheetId="0">Sheet1!$A$1:$AJ$19</definedName>
+    <definedName name="merged_part2q1_out" localSheetId="0">'1a'!$A$1:$AJ$19</definedName>
+    <definedName name="merged_part2q2_c32" localSheetId="2">'2a chunk32'!$A$1:$AJ$11</definedName>
+    <definedName name="merged_part2q2_c64" localSheetId="1">'2a chunk64'!$A$1:$AJ$11</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -65,11 +69,95 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="merged_part2q2_c32.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:jacqueline.lo:Documents:classes:eem116c:eem116c-project:part2:merged_part2q2_c32.csv" comma="1">
+      <textFields count="36">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="merged_part2q2_c64.csv" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:jacqueline.lo:Documents:classes:eem116c:eem116c-project:part2:merged_part2q2_c64.csv" comma="1">
+      <textFields count="36">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="42">
   <si>
     <t>Test Name</t>
   </si>
@@ -187,15 +275,43 @@
   <si>
     <t>ns/access</t>
   </si>
+  <si>
+    <t>Test #1T (Throughput)</t>
+  </si>
+  <si>
+    <t>SEQUENTIAL</t>
+  </si>
+  <si>
+    <t>READ</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -218,14 +334,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -268,7 +389,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -282,7 +402,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$1</c:f>
+              <c:f>'1a'!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -296,9 +416,9 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$19</c:f>
+              <c:f>'1a'!$C$2:$C$19</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
                   <c:v>4.0</c:v>
@@ -359,7 +479,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$2:$V$19</c:f>
+              <c:f>'1a'!$V$2:$V$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -432,11 +552,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137851240"/>
-        <c:axId val="-2142288440"/>
+        <c:axId val="2069829208"/>
+        <c:axId val="2069653816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137851240"/>
+        <c:axId val="2069829208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -463,14 +583,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2142288440"/>
+        <c:crossAx val="2069653816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -478,7 +597,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2142288440"/>
+        <c:axId val="2069653816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -506,20 +625,495 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137851240"/>
+        <c:crossAx val="2069829208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Throughput</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Stride Length</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (chunk size 64 bits)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2a chunk64'!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2a chunk64'!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>42411.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49471.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44627.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47252.7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46441.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43346.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>50068.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45028.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41625.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44303.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2108055400"/>
+        <c:axId val="-2051957048"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2108055400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stride</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2051957048"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2051957048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Throughput (MB/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2108055400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Throughput</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Stride Length</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> (chunk size 32 bits)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2a chunk64'!$K$2:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-16.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2a chunk32'!$L$2:$L$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>22893.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21836.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22422.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21821.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24022.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23681.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23272.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21078.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21510.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21852.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2107658776"/>
+        <c:axId val="-2138424696"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2107658776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stride</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2138424696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2138424696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Mean Throughput (MB/s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2107658776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
@@ -567,8 +1161,88 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1498600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="merged_part2q1_out" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="merged_part2q2_c64" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="merged_part2q2_c32" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1048,7 +1722,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>4</v>
       </c>
       <c r="D2">
@@ -1152,7 +1826,7 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>8</v>
       </c>
       <c r="D3">
@@ -1256,7 +1930,7 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>16</v>
       </c>
       <c r="D4">
@@ -1360,7 +2034,7 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>32</v>
       </c>
       <c r="D5">
@@ -1464,7 +2138,7 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>64</v>
       </c>
       <c r="D6">
@@ -1568,7 +2242,7 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>128</v>
       </c>
       <c r="D7">
@@ -1672,7 +2346,7 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>256</v>
       </c>
       <c r="D8">
@@ -1776,7 +2450,7 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>512</v>
       </c>
       <c r="D9">
@@ -1880,7 +2554,7 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>1024</v>
       </c>
       <c r="D10">
@@ -1984,7 +2658,7 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>2048</v>
       </c>
       <c r="D11">
@@ -2088,7 +2762,7 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>4096</v>
       </c>
       <c r="D12">
@@ -2192,7 +2866,7 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>8192</v>
       </c>
       <c r="D13">
@@ -2296,7 +2970,7 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>16384</v>
       </c>
       <c r="D14">
@@ -2400,7 +3074,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>32768</v>
       </c>
       <c r="D15">
@@ -2504,7 +3178,7 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>65536</v>
       </c>
       <c r="D16">
@@ -2608,7 +3282,7 @@
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>131072</v>
       </c>
       <c r="D17">
@@ -2712,7 +3386,7 @@
       <c r="B18">
         <v>1</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>262144</v>
       </c>
       <c r="D18">
@@ -2816,7 +3490,7 @@
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>524288</v>
       </c>
       <c r="D19">
@@ -2926,4 +3600,2413 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2">
+        <v>64</v>
+      </c>
+      <c r="K2" s="2">
+        <v>-16</v>
+      </c>
+      <c r="L2" s="1">
+        <v>42411.4</v>
+      </c>
+      <c r="M2">
+        <v>42411.4</v>
+      </c>
+      <c r="N2">
+        <v>42411.4</v>
+      </c>
+      <c r="O2">
+        <v>42411.4</v>
+      </c>
+      <c r="P2">
+        <v>42411.4</v>
+      </c>
+      <c r="Q2">
+        <v>42411.4</v>
+      </c>
+      <c r="R2">
+        <v>42411.4</v>
+      </c>
+      <c r="S2">
+        <v>42411.4</v>
+      </c>
+      <c r="T2">
+        <v>42411.4</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35" ht="16" customHeight="1">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3">
+        <v>64</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-8</v>
+      </c>
+      <c r="L3" s="1">
+        <v>49471.6</v>
+      </c>
+      <c r="M3">
+        <v>49471.6</v>
+      </c>
+      <c r="N3">
+        <v>49471.6</v>
+      </c>
+      <c r="O3">
+        <v>49471.6</v>
+      </c>
+      <c r="P3">
+        <v>49471.6</v>
+      </c>
+      <c r="Q3">
+        <v>49471.6</v>
+      </c>
+      <c r="R3">
+        <v>49471.6</v>
+      </c>
+      <c r="S3">
+        <v>49471.6</v>
+      </c>
+      <c r="T3">
+        <v>49471.6</v>
+      </c>
+      <c r="U3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4">
+        <v>64</v>
+      </c>
+      <c r="K4" s="2">
+        <v>-4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>44627.4</v>
+      </c>
+      <c r="M4">
+        <v>44627.4</v>
+      </c>
+      <c r="N4">
+        <v>44627.4</v>
+      </c>
+      <c r="O4">
+        <v>44627.4</v>
+      </c>
+      <c r="P4">
+        <v>44627.4</v>
+      </c>
+      <c r="Q4">
+        <v>44627.4</v>
+      </c>
+      <c r="R4">
+        <v>44627.4</v>
+      </c>
+      <c r="S4">
+        <v>44627.4</v>
+      </c>
+      <c r="T4">
+        <v>44627.4</v>
+      </c>
+      <c r="U4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>64</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>47252.7</v>
+      </c>
+      <c r="M5">
+        <v>47252.7</v>
+      </c>
+      <c r="N5">
+        <v>47252.7</v>
+      </c>
+      <c r="O5">
+        <v>47252.7</v>
+      </c>
+      <c r="P5">
+        <v>47252.7</v>
+      </c>
+      <c r="Q5">
+        <v>47252.7</v>
+      </c>
+      <c r="R5">
+        <v>47252.7</v>
+      </c>
+      <c r="S5">
+        <v>47252.7</v>
+      </c>
+      <c r="T5">
+        <v>47252.7</v>
+      </c>
+      <c r="U5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6">
+        <v>64</v>
+      </c>
+      <c r="K6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>46441.1</v>
+      </c>
+      <c r="M6">
+        <v>46441.1</v>
+      </c>
+      <c r="N6">
+        <v>46441.1</v>
+      </c>
+      <c r="O6">
+        <v>46441.1</v>
+      </c>
+      <c r="P6">
+        <v>46441.1</v>
+      </c>
+      <c r="Q6">
+        <v>46441.1</v>
+      </c>
+      <c r="R6">
+        <v>46441.1</v>
+      </c>
+      <c r="S6">
+        <v>46441.1</v>
+      </c>
+      <c r="T6">
+        <v>46441.1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7">
+        <v>64</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>43346.6</v>
+      </c>
+      <c r="M7">
+        <v>43346.6</v>
+      </c>
+      <c r="N7">
+        <v>43346.6</v>
+      </c>
+      <c r="O7">
+        <v>43346.6</v>
+      </c>
+      <c r="P7">
+        <v>43346.6</v>
+      </c>
+      <c r="Q7">
+        <v>43346.6</v>
+      </c>
+      <c r="R7">
+        <v>43346.6</v>
+      </c>
+      <c r="S7">
+        <v>43346.6</v>
+      </c>
+      <c r="T7">
+        <v>43346.6</v>
+      </c>
+      <c r="U7" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8">
+        <v>64</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>50068.1</v>
+      </c>
+      <c r="M8">
+        <v>50068.1</v>
+      </c>
+      <c r="N8">
+        <v>50068.1</v>
+      </c>
+      <c r="O8">
+        <v>50068.1</v>
+      </c>
+      <c r="P8">
+        <v>50068.1</v>
+      </c>
+      <c r="Q8">
+        <v>50068.1</v>
+      </c>
+      <c r="R8">
+        <v>50068.1</v>
+      </c>
+      <c r="S8">
+        <v>50068.1</v>
+      </c>
+      <c r="T8">
+        <v>50068.1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9">
+        <v>64</v>
+      </c>
+      <c r="K9" s="2">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
+        <v>45028.4</v>
+      </c>
+      <c r="M9">
+        <v>45028.4</v>
+      </c>
+      <c r="N9">
+        <v>45028.4</v>
+      </c>
+      <c r="O9">
+        <v>45028.4</v>
+      </c>
+      <c r="P9">
+        <v>45028.4</v>
+      </c>
+      <c r="Q9">
+        <v>45028.4</v>
+      </c>
+      <c r="R9">
+        <v>45028.4</v>
+      </c>
+      <c r="S9">
+        <v>45028.4</v>
+      </c>
+      <c r="T9">
+        <v>45028.4</v>
+      </c>
+      <c r="U9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10">
+        <v>64</v>
+      </c>
+      <c r="K10" s="2">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="M10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="N10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="O10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="P10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="Q10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="R10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="S10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="T10">
+        <v>41625.300000000003</v>
+      </c>
+      <c r="U10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11">
+        <v>64</v>
+      </c>
+      <c r="K11" s="2">
+        <v>16</v>
+      </c>
+      <c r="L11" s="1">
+        <v>44303</v>
+      </c>
+      <c r="M11">
+        <v>44303</v>
+      </c>
+      <c r="N11">
+        <v>44303</v>
+      </c>
+      <c r="O11">
+        <v>44303</v>
+      </c>
+      <c r="P11">
+        <v>44303</v>
+      </c>
+      <c r="Q11">
+        <v>44303</v>
+      </c>
+      <c r="R11">
+        <v>44303</v>
+      </c>
+      <c r="S11">
+        <v>44303</v>
+      </c>
+      <c r="T11">
+        <v>44303</v>
+      </c>
+      <c r="U11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" t="s">
+        <v>36</v>
+      </c>
+      <c r="W11" t="s">
+        <v>36</v>
+      </c>
+      <c r="X11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:AI11">
+    <sortCondition ref="K2:K11"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="31" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="19" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2">
+        <v>32</v>
+      </c>
+      <c r="K2" s="2">
+        <v>-16</v>
+      </c>
+      <c r="L2" s="1">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="M2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="N2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="O2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="P2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="Q2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="R2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="S2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="T2">
+        <v>22893.599999999999</v>
+      </c>
+      <c r="U2" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:35">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3">
+        <v>32</v>
+      </c>
+      <c r="K3" s="2">
+        <v>-8</v>
+      </c>
+      <c r="L3" s="1">
+        <v>21836.5</v>
+      </c>
+      <c r="M3">
+        <v>21836.5</v>
+      </c>
+      <c r="N3">
+        <v>21836.5</v>
+      </c>
+      <c r="O3">
+        <v>21836.5</v>
+      </c>
+      <c r="P3">
+        <v>21836.5</v>
+      </c>
+      <c r="Q3">
+        <v>21836.5</v>
+      </c>
+      <c r="R3">
+        <v>21836.5</v>
+      </c>
+      <c r="S3">
+        <v>21836.5</v>
+      </c>
+      <c r="T3">
+        <v>21836.5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" t="s">
+        <v>36</v>
+      </c>
+      <c r="X3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4">
+        <v>32</v>
+      </c>
+      <c r="K4" s="2">
+        <v>-4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>22422.3</v>
+      </c>
+      <c r="M4">
+        <v>22422.3</v>
+      </c>
+      <c r="N4">
+        <v>22422.3</v>
+      </c>
+      <c r="O4">
+        <v>22422.3</v>
+      </c>
+      <c r="P4">
+        <v>22422.3</v>
+      </c>
+      <c r="Q4">
+        <v>22422.3</v>
+      </c>
+      <c r="R4">
+        <v>22422.3</v>
+      </c>
+      <c r="S4">
+        <v>22422.3</v>
+      </c>
+      <c r="T4">
+        <v>22422.3</v>
+      </c>
+      <c r="U4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V4" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5">
+        <v>32</v>
+      </c>
+      <c r="K5" s="2">
+        <v>-2</v>
+      </c>
+      <c r="L5" s="1">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="M5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="N5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="O5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="P5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="Q5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="R5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="S5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="T5">
+        <v>21821.200000000001</v>
+      </c>
+      <c r="U5" t="s">
+        <v>37</v>
+      </c>
+      <c r="V5" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" t="s">
+        <v>36</v>
+      </c>
+      <c r="X5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF5">
+        <v>0</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6">
+        <v>32</v>
+      </c>
+      <c r="K6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>24022.3</v>
+      </c>
+      <c r="M6">
+        <v>24022.3</v>
+      </c>
+      <c r="N6">
+        <v>24022.3</v>
+      </c>
+      <c r="O6">
+        <v>24022.3</v>
+      </c>
+      <c r="P6">
+        <v>24022.3</v>
+      </c>
+      <c r="Q6">
+        <v>24022.3</v>
+      </c>
+      <c r="R6">
+        <v>24022.3</v>
+      </c>
+      <c r="S6">
+        <v>24022.3</v>
+      </c>
+      <c r="T6">
+        <v>24022.3</v>
+      </c>
+      <c r="U6" t="s">
+        <v>37</v>
+      </c>
+      <c r="V6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7">
+        <v>32</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="1">
+        <v>23681.3</v>
+      </c>
+      <c r="M7">
+        <v>23681.3</v>
+      </c>
+      <c r="N7">
+        <v>23681.3</v>
+      </c>
+      <c r="O7">
+        <v>23681.3</v>
+      </c>
+      <c r="P7">
+        <v>23681.3</v>
+      </c>
+      <c r="Q7">
+        <v>23681.3</v>
+      </c>
+      <c r="R7">
+        <v>23681.3</v>
+      </c>
+      <c r="S7">
+        <v>23681.3</v>
+      </c>
+      <c r="T7">
+        <v>23681.3</v>
+      </c>
+      <c r="U7" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" t="s">
+        <v>36</v>
+      </c>
+      <c r="W7" t="s">
+        <v>36</v>
+      </c>
+      <c r="X7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:35">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8">
+        <v>32</v>
+      </c>
+      <c r="K8" s="2">
+        <v>2</v>
+      </c>
+      <c r="L8" s="1">
+        <v>23272.6</v>
+      </c>
+      <c r="M8">
+        <v>23272.6</v>
+      </c>
+      <c r="N8">
+        <v>23272.6</v>
+      </c>
+      <c r="O8">
+        <v>23272.6</v>
+      </c>
+      <c r="P8">
+        <v>23272.6</v>
+      </c>
+      <c r="Q8">
+        <v>23272.6</v>
+      </c>
+      <c r="R8">
+        <v>23272.6</v>
+      </c>
+      <c r="S8">
+        <v>23272.6</v>
+      </c>
+      <c r="T8">
+        <v>23272.6</v>
+      </c>
+      <c r="U8" t="s">
+        <v>37</v>
+      </c>
+      <c r="V8" t="s">
+        <v>36</v>
+      </c>
+      <c r="W8" t="s">
+        <v>36</v>
+      </c>
+      <c r="X8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF8">
+        <v>0</v>
+      </c>
+      <c r="AG8">
+        <v>0</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:35">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9">
+        <v>32</v>
+      </c>
+      <c r="K9" s="2">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="M9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="N9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="O9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="P9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="Q9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="R9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="S9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="T9">
+        <v>21078.799999999999</v>
+      </c>
+      <c r="U9" t="s">
+        <v>37</v>
+      </c>
+      <c r="V9" t="s">
+        <v>36</v>
+      </c>
+      <c r="W9" t="s">
+        <v>36</v>
+      </c>
+      <c r="X9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF9">
+        <v>0</v>
+      </c>
+      <c r="AG9">
+        <v>0</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10">
+        <v>32</v>
+      </c>
+      <c r="K10" s="2">
+        <v>8</v>
+      </c>
+      <c r="L10" s="1">
+        <v>21510.9</v>
+      </c>
+      <c r="M10">
+        <v>21510.9</v>
+      </c>
+      <c r="N10">
+        <v>21510.9</v>
+      </c>
+      <c r="O10">
+        <v>21510.9</v>
+      </c>
+      <c r="P10">
+        <v>21510.9</v>
+      </c>
+      <c r="Q10">
+        <v>21510.9</v>
+      </c>
+      <c r="R10">
+        <v>21510.9</v>
+      </c>
+      <c r="S10">
+        <v>21510.9</v>
+      </c>
+      <c r="T10">
+        <v>21510.9</v>
+      </c>
+      <c r="U10" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" t="s">
+        <v>36</v>
+      </c>
+      <c r="W10" t="s">
+        <v>36</v>
+      </c>
+      <c r="X10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF10">
+        <v>0</v>
+      </c>
+      <c r="AG10">
+        <v>0</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11">
+        <v>32</v>
+      </c>
+      <c r="K11" s="2">
+        <v>16</v>
+      </c>
+      <c r="L11" s="1">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="M11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="N11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="O11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="P11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="Q11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="R11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="S11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="T11">
+        <v>21852.799999999999</v>
+      </c>
+      <c r="U11" t="s">
+        <v>37</v>
+      </c>
+      <c r="V11" t="s">
+        <v>36</v>
+      </c>
+      <c r="W11" t="s">
+        <v>36</v>
+      </c>
+      <c r="X11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:AI11">
+    <sortCondition ref="K2:K11"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>